<commit_message>
made changes to test files, made missing gene name test file
</commit_message>
<xml_diff>
--- a/test-files/gene-name-modifications/duplicate-gene-side-and-top-nonadjacent-input.xlsx
+++ b/test-files/gene-name-modifications/duplicate-gene-side-and-top-nonadjacent-input.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26311"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mihir/Documents/School/GRNsight/test-files/gene-name-modifications/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14160" tabRatio="759" firstSheet="6" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14160" tabRatio="759" firstSheet="6" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,12 +18,7 @@
     <sheet name="log2_concentrations" sheetId="4" r:id="rId4"/>
     <sheet name="log2_optimized_concentrations" sheetId="5" r:id="rId5"/>
     <sheet name="degradation_rates" sheetId="6" r:id="rId6"/>
-    <sheet name="production_rates" sheetId="7" r:id="rId7"/>
-    <sheet name="measurement_times" sheetId="8" r:id="rId8"/>
-    <sheet name="network" sheetId="9" r:id="rId9"/>
-    <sheet name="network_weights" sheetId="10" r:id="rId10"/>
-    <sheet name="network_optimized_b" sheetId="11" r:id="rId11"/>
-    <sheet name="concentration_sigmas" sheetId="13" r:id="rId12"/>
+    <sheet name="network" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="46">
   <si>
     <t>SystematicName</t>
   </si>
@@ -167,16 +167,7 @@
     <t>DegradationRate</t>
   </si>
   <si>
-    <t>production_rates</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>rows genes affected/cols genes controlling</t>
-  </si>
-  <si>
-    <t>b</t>
+    <t>`</t>
   </si>
 </sst>
 </file>
@@ -296,6 +287,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -625,2186 +621,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:22">
-      <c r="A1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M1" t="s">
-        <v>25</v>
-      </c>
-      <c r="N1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P1" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>33</v>
-      </c>
-      <c r="R1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S1" t="s">
-        <v>37</v>
-      </c>
-      <c r="T1" t="s">
-        <v>39</v>
-      </c>
-      <c r="U1" t="s">
-        <v>41</v>
-      </c>
-      <c r="V1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2">
-        <v>0</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-      <c r="V2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>1</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>1</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3">
-        <v>0</v>
-      </c>
-      <c r="U3">
-        <v>0</v>
-      </c>
-      <c r="V3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4">
-        <v>0</v>
-      </c>
-      <c r="U4">
-        <v>0</v>
-      </c>
-      <c r="V4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-      <c r="V5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6">
-        <v>0</v>
-      </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
-      <c r="V6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>1</v>
-      </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-      <c r="T7">
-        <v>0</v>
-      </c>
-      <c r="U7">
-        <v>0</v>
-      </c>
-      <c r="V7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8">
-        <v>0</v>
-      </c>
-      <c r="U8">
-        <v>1</v>
-      </c>
-      <c r="V8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-      <c r="R9">
-        <v>0</v>
-      </c>
-      <c r="S9">
-        <v>0</v>
-      </c>
-      <c r="T9">
-        <v>0</v>
-      </c>
-      <c r="U9">
-        <v>0</v>
-      </c>
-      <c r="V9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-      <c r="R10">
-        <v>0</v>
-      </c>
-      <c r="S10">
-        <v>0</v>
-      </c>
-      <c r="T10">
-        <v>0</v>
-      </c>
-      <c r="U10">
-        <v>0</v>
-      </c>
-      <c r="V10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-      <c r="R11">
-        <v>0</v>
-      </c>
-      <c r="S11">
-        <v>0</v>
-      </c>
-      <c r="T11">
-        <v>0</v>
-      </c>
-      <c r="U11">
-        <v>0</v>
-      </c>
-      <c r="V11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>1</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12">
-        <v>0</v>
-      </c>
-      <c r="Q12">
-        <v>0</v>
-      </c>
-      <c r="R12">
-        <v>0</v>
-      </c>
-      <c r="S12">
-        <v>0</v>
-      </c>
-      <c r="T12">
-        <v>0</v>
-      </c>
-      <c r="U12">
-        <v>0</v>
-      </c>
-      <c r="V12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22">
-      <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13">
-        <v>1</v>
-      </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-      <c r="P13">
-        <v>0</v>
-      </c>
-      <c r="Q13">
-        <v>0</v>
-      </c>
-      <c r="R13">
-        <v>0</v>
-      </c>
-      <c r="S13">
-        <v>0</v>
-      </c>
-      <c r="T13">
-        <v>0</v>
-      </c>
-      <c r="U13">
-        <v>1</v>
-      </c>
-      <c r="V13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22">
-      <c r="A14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
-      <c r="N14">
-        <v>0</v>
-      </c>
-      <c r="O14">
-        <v>1</v>
-      </c>
-      <c r="P14">
-        <v>0</v>
-      </c>
-      <c r="Q14">
-        <v>0</v>
-      </c>
-      <c r="R14">
-        <v>0</v>
-      </c>
-      <c r="S14">
-        <v>0</v>
-      </c>
-      <c r="T14">
-        <v>0</v>
-      </c>
-      <c r="U14">
-        <v>0</v>
-      </c>
-      <c r="V14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22">
-      <c r="A15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-      <c r="N15">
-        <v>0</v>
-      </c>
-      <c r="O15">
-        <v>0</v>
-      </c>
-      <c r="P15">
-        <v>1</v>
-      </c>
-      <c r="Q15">
-        <v>0</v>
-      </c>
-      <c r="R15">
-        <v>0</v>
-      </c>
-      <c r="S15">
-        <v>0</v>
-      </c>
-      <c r="T15">
-        <v>0</v>
-      </c>
-      <c r="U15">
-        <v>0</v>
-      </c>
-      <c r="V15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22">
-      <c r="A16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>1</v>
-      </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16">
-        <v>0</v>
-      </c>
-      <c r="M16">
-        <v>0</v>
-      </c>
-      <c r="N16">
-        <v>0</v>
-      </c>
-      <c r="O16">
-        <v>0</v>
-      </c>
-      <c r="P16">
-        <v>0</v>
-      </c>
-      <c r="Q16">
-        <v>0</v>
-      </c>
-      <c r="R16">
-        <v>1</v>
-      </c>
-      <c r="S16">
-        <v>1</v>
-      </c>
-      <c r="T16">
-        <v>0</v>
-      </c>
-      <c r="U16">
-        <v>0</v>
-      </c>
-      <c r="V16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22">
-      <c r="A17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>1</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17">
-        <v>0</v>
-      </c>
-      <c r="N17">
-        <v>0</v>
-      </c>
-      <c r="O17">
-        <v>0</v>
-      </c>
-      <c r="P17">
-        <v>0</v>
-      </c>
-      <c r="Q17">
-        <v>0</v>
-      </c>
-      <c r="R17">
-        <v>0</v>
-      </c>
-      <c r="S17">
-        <v>0</v>
-      </c>
-      <c r="T17">
-        <v>0</v>
-      </c>
-      <c r="U17">
-        <v>0</v>
-      </c>
-      <c r="V17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22">
-      <c r="A18" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
-      <c r="N18">
-        <v>0</v>
-      </c>
-      <c r="O18">
-        <v>0</v>
-      </c>
-      <c r="P18">
-        <v>1</v>
-      </c>
-      <c r="Q18">
-        <v>0</v>
-      </c>
-      <c r="R18">
-        <v>0</v>
-      </c>
-      <c r="S18">
-        <v>0</v>
-      </c>
-      <c r="T18">
-        <v>0</v>
-      </c>
-      <c r="U18">
-        <v>0</v>
-      </c>
-      <c r="V18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22">
-      <c r="A19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="J19">
-        <v>1</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
-      <c r="N19">
-        <v>0</v>
-      </c>
-      <c r="O19">
-        <v>0</v>
-      </c>
-      <c r="P19">
-        <v>0</v>
-      </c>
-      <c r="Q19">
-        <v>0</v>
-      </c>
-      <c r="R19">
-        <v>0</v>
-      </c>
-      <c r="S19">
-        <v>0</v>
-      </c>
-      <c r="T19">
-        <v>0</v>
-      </c>
-      <c r="U19">
-        <v>0</v>
-      </c>
-      <c r="V19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22">
-      <c r="A20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="K20">
-        <v>1</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-      <c r="M20">
-        <v>0</v>
-      </c>
-      <c r="N20">
-        <v>0</v>
-      </c>
-      <c r="O20">
-        <v>0</v>
-      </c>
-      <c r="P20">
-        <v>0</v>
-      </c>
-      <c r="Q20">
-        <v>0</v>
-      </c>
-      <c r="R20">
-        <v>1</v>
-      </c>
-      <c r="S20">
-        <v>0</v>
-      </c>
-      <c r="T20">
-        <v>0</v>
-      </c>
-      <c r="U20">
-        <v>0</v>
-      </c>
-      <c r="V20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22">
-      <c r="A21" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-      <c r="M21">
-        <v>0</v>
-      </c>
-      <c r="N21">
-        <v>0</v>
-      </c>
-      <c r="O21">
-        <v>0</v>
-      </c>
-      <c r="P21">
-        <v>0</v>
-      </c>
-      <c r="Q21">
-        <v>0</v>
-      </c>
-      <c r="R21">
-        <v>0</v>
-      </c>
-      <c r="S21">
-        <v>0</v>
-      </c>
-      <c r="T21">
-        <v>1</v>
-      </c>
-      <c r="U21">
-        <v>1</v>
-      </c>
-      <c r="V21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22">
-      <c r="A22" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
-      <c r="M22">
-        <v>0</v>
-      </c>
-      <c r="N22">
-        <v>0</v>
-      </c>
-      <c r="O22">
-        <v>0</v>
-      </c>
-      <c r="P22">
-        <v>0</v>
-      </c>
-      <c r="Q22">
-        <v>0</v>
-      </c>
-      <c r="R22">
-        <v>0</v>
-      </c>
-      <c r="S22">
-        <v>0</v>
-      </c>
-      <c r="T22">
-        <v>0</v>
-      </c>
-      <c r="U22">
-        <v>0</v>
-      </c>
-      <c r="V22">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>0.6791483455907944</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>0.48264401872948809</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5">
-        <v>3.1789251600063162</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7">
-        <v>2.9142418243700741</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8">
-        <v>2.747116954400004</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11">
-        <v>1.3234711509044375</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12">
-        <v>2.3716065337281029</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13">
-        <v>1.062252458233609</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14">
-        <v>2.8050668756259403</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15">
-        <v>1.4681065483366496</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16">
-        <v>6.652945086765409</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17">
-        <v>0.6334178159085323</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18">
-        <v>0.44122959808620299</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19">
-        <v>2.6942167728845008</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20">
-        <v>2.090174007095754</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21">
-        <v>0.66239849617041691</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>15</v>
-      </c>
-      <c r="D1">
-        <v>30</v>
-      </c>
-      <c r="E1">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>0.91727409105065705</v>
-      </c>
-      <c r="D2">
-        <v>0.44210879486447602</v>
-      </c>
-      <c r="E2">
-        <v>0.69315515241602899</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>0.71685637353245302</v>
-      </c>
-      <c r="D3">
-        <v>0.641384013885964</v>
-      </c>
-      <c r="E3">
-        <v>0.92245951116837099</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>0.44470247868505602</v>
-      </c>
-      <c r="D4">
-        <v>0.53164120946850402</v>
-      </c>
-      <c r="E4">
-        <v>0.320493749001932</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5">
-        <v>0.81727687981679498</v>
-      </c>
-      <c r="D5">
-        <v>0.95726655288635398</v>
-      </c>
-      <c r="E5">
-        <v>0.70281582595053704</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6">
-        <v>1.0967850406720701</v>
-      </c>
-      <c r="D6">
-        <v>0.52970920759899298</v>
-      </c>
-      <c r="E6">
-        <v>0.80891828959740097</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7">
-        <v>0.42580145197082703</v>
-      </c>
-      <c r="D7">
-        <v>0.63499396842678302</v>
-      </c>
-      <c r="E7">
-        <v>0.78157727034137603</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8">
-        <v>0.404638632823907</v>
-      </c>
-      <c r="D8">
-        <v>0.58989131883839296</v>
-      </c>
-      <c r="E8">
-        <v>0.60748498565234699</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9">
-        <v>0.68943520086600596</v>
-      </c>
-      <c r="D9">
-        <v>1.8955428214225301</v>
-      </c>
-      <c r="E9">
-        <v>0.54723644512184799</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10">
-        <v>0.97726406268218102</v>
-      </c>
-      <c r="D10">
-        <v>0.72420652572711597</v>
-      </c>
-      <c r="E10">
-        <v>1.09985790153451</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11">
-        <v>0.72504670083612599</v>
-      </c>
-      <c r="D11">
-        <v>0.20779307950352699</v>
-      </c>
-      <c r="E11">
-        <v>0.65825511050072905</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12">
-        <v>0.51852196117730698</v>
-      </c>
-      <c r="D12">
-        <v>0.88709656674279203</v>
-      </c>
-      <c r="E12">
-        <v>0.248881921070051</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13">
-        <v>1.6409513470958299</v>
-      </c>
-      <c r="D13">
-        <v>1.01226276719667</v>
-      </c>
-      <c r="E13">
-        <v>1.2436321609087699</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14">
-        <v>0.56438763790471502</v>
-      </c>
-      <c r="D14">
-        <v>0.637046148638169</v>
-      </c>
-      <c r="E14">
-        <v>0.76246682595887705</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15">
-        <v>0.48729361226630702</v>
-      </c>
-      <c r="D15">
-        <v>0.460208681767377</v>
-      </c>
-      <c r="E15">
-        <v>0.389622153973187</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16">
-        <v>1.72099674768658</v>
-      </c>
-      <c r="D16">
-        <v>0.85831878781873805</v>
-      </c>
-      <c r="E16">
-        <v>0.44772738659776701</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17">
-        <v>0.50452893050955805</v>
-      </c>
-      <c r="D17">
-        <v>0.75370009518917203</v>
-      </c>
-      <c r="E17">
-        <v>1.07122097617887</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18">
-        <v>1.1966265259256601</v>
-      </c>
-      <c r="D18">
-        <v>1.1801382981458799</v>
-      </c>
-      <c r="E18">
-        <v>0.35000209622478101</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19">
-        <v>1.48156426614991</v>
-      </c>
-      <c r="D19">
-        <v>1.7277862291131501</v>
-      </c>
-      <c r="E19">
-        <v>0.89902628670097295</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20">
-        <v>1.10568541431009</v>
-      </c>
-      <c r="D20">
-        <v>0.84212726958299999</v>
-      </c>
-      <c r="E20">
-        <v>0.74688657635395606</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21">
-        <v>0.65898902973629203</v>
-      </c>
-      <c r="D21">
-        <v>0.43418451003840802</v>
-      </c>
-      <c r="E21">
-        <v>0.53794081650927705</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22">
-        <v>0.40923963868872798</v>
-      </c>
-      <c r="D22">
-        <v>0.28048461336490499</v>
-      </c>
-      <c r="E22">
-        <v>0.287254982132019</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2814,14 +633,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2831,14 +645,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2850,9 +659,9 @@
       <selection sqref="A1:E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2869,7 +678,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2886,7 +695,7 @@
         <v>-2.2843447109758301</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2903,7 +712,7 @@
         <v>-8.4072251269262696E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2920,7 +729,7 @@
         <v>0.29611171632314098</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2937,7 +746,7 @@
         <v>1.75845186354745</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -2954,7 +763,7 @@
         <v>-0.76236366760055096</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -2971,7 +780,7 @@
         <v>0.62853290835895503</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2988,7 +797,7 @@
         <v>-8.7143718210927298E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -3005,7 +814,7 @@
         <v>0.84698244904192099</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -3022,7 +831,7 @@
         <v>-0.73218305564943398</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -3039,7 +848,7 @@
         <v>0.45176478094112998</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -3056,7 +865,7 @@
         <v>-0.48116619434522001</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -3073,7 +882,7 @@
         <v>1.4416179829439899</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -3090,7 +899,7 @@
         <v>-0.29043031142040199</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -3107,7 +916,7 @@
         <v>0.41039596022329999</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -3124,7 +933,7 @@
         <v>9.0586658239791298E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -3141,7 +950,7 @@
         <v>-0.19878651280399501</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -3158,7 +967,7 @@
         <v>-1.1921015273515501</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -3175,7 +984,7 @@
         <v>1.5309831587774501</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -3192,7 +1001,7 @@
         <v>1.4171295501935499</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -3209,7 +1018,7 @@
         <v>1.50806209670647</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -3228,11 +1037,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3244,9 +1048,9 @@
       <selection sqref="A1:I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3275,7 +1079,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -3304,7 +1108,7 @@
         <v>-1.614737262334736</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -3333,7 +1137,7 @@
         <v>-4.4152407880423003E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -3362,7 +1166,7 @@
         <v>0.34245532652126665</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -3391,7 +1195,7 @@
         <v>1.5632943329859523</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -3420,7 +1224,7 @@
         <v>-0.98278112783760696</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -3449,7 +1253,7 @@
         <v>0.61518119934801141</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -3478,7 +1282,7 @@
         <v>-0.134864828008146</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -3507,7 +1311,7 @@
         <v>0.52007384366239306</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -3536,7 +1340,7 @@
         <v>-1.1238172749525641</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -3565,7 +1369,7 @@
         <v>0.62289346498752207</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -3594,7 +1398,7 @@
         <v>-0.40518417542879076</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -3623,7 +1427,7 @@
         <v>1.3857553092197141</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -3652,7 +1456,7 @@
         <v>-0.32348780752512174</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -3681,7 +1485,7 @@
         <v>0.59223490664700296</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -3710,7 +1514,7 @@
         <v>7.2760038315940578E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -3739,7 +1543,7 @@
         <v>-0.2313321871712328</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -3768,7 +1572,7 @@
         <v>-1.153846153117154</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -3797,7 +1601,7 @@
         <v>1.7594447626156464</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -3826,7 +1630,7 @@
         <v>1.3835119382868828</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -3855,7 +1659,7 @@
         <v>1.4505220392146478</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -3886,11 +1690,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3902,9 +1701,9 @@
       <selection sqref="A1:C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3915,7 +1714,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -3926,7 +1725,7 @@
         <v>0.34657359027997264</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -3937,7 +1736,7 @@
         <v>0.23104906018664842</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -3948,7 +1747,7 @@
         <v>3.0136833937388925E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -3959,7 +1758,7 @@
         <v>2.7179999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -3970,7 +1769,7 @@
         <v>2.5672117798516494E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -3981,7 +1780,7 @@
         <v>1.7328679513998631E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -3992,7 +1791,7 @@
         <v>1.1002336199364211E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -4003,7 +1802,7 @@
         <v>2.7179999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -4014,7 +1813,7 @@
         <v>2.7179999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -4025,7 +1824,7 @@
         <v>7.453195489891885E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -4036,7 +1835,7 @@
         <v>7.7016353395549478E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -4047,7 +1846,7 @@
         <v>2.7179999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -4058,7 +1857,7 @@
         <v>6.9314718055994526E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -4069,7 +1868,7 @@
         <v>4.9510512897138946E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -4080,7 +1879,7 @@
         <v>1.6503504299046318E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -4091,7 +1890,7 @@
         <v>5.7762265046662105E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -4102,7 +1901,7 @@
         <v>1.332975347230664E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -4113,7 +1912,7 @@
         <v>1.2602676010180823E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -4124,7 +1923,7 @@
         <v>3.0136833937388925E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -4135,7 +1934,7 @@
         <v>3.0136833937388925E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -4148,323 +1947,22 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>0.22632946888165298</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>0.95204138649003045</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>0.10226183333718407</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5">
-        <v>0.67232014103810334</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6">
-        <v>1.9061895013331151E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7">
-        <v>0.23622212585757982</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8">
-        <v>7.7673277547578606E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9">
-        <v>8.3697232288375042E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10">
-        <v>1.7784026774789942E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11">
-        <v>0.28919483541793922</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12">
-        <v>0.4504418743837888</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13">
-        <v>0.46107669765430792</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14">
-        <v>0.54348364788398873</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15">
-        <v>0.5005684311220312</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16">
-        <v>0.29329211144014761</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17">
-        <v>0.14136838611674404</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19">
-        <v>0.65407775836354121</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20">
-        <v>0.55800134575802074</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21">
-        <v>1.109523323046905</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22">
-        <v>3.3009606163385587E-2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1">
-        <v>15</v>
-      </c>
-      <c r="C1">
-        <v>30</v>
-      </c>
-      <c r="D1">
-        <v>60</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
@@ -4473,19 +1971,19 @@
         <v>5</v>
       </c>
       <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>13</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
       </c>
       <c r="I1" t="s">
         <v>15</v>
@@ -4533,7 +2031,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4604,7 +2102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -4615,10 +2113,10 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -4675,7 +2173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -4686,7 +2184,7 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -4698,7 +2196,7 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -4746,7 +2244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -4817,7 +2315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -4888,7 +2386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -4902,10 +2400,10 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -4959,7 +2457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -4970,10 +2468,10 @@
         <v>0</v>
       </c>
       <c r="D8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="1">
         <v>0</v>
@@ -5030,7 +2528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -5101,7 +2599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -5172,7 +2670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -5243,7 +2741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -5257,10 +2755,10 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -5314,7 +2812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:23">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -5385,7 +2883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:23">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -5405,10 +2903,10 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14">
         <v>0</v>
@@ -5456,7 +2954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -5473,10 +2971,10 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -5527,7 +3025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:23">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -5598,7 +3096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:23">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -5669,7 +3167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:23">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -5740,7 +3238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:23">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -5751,10 +3249,10 @@
         <v>0</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -5811,7 +3309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:23">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -5882,7 +3380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:23">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -5953,7 +3451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:23">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -6024,7 +3522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:23">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -6098,10 +3596,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>